<commit_message>
Update 15-Mar-2021, beginning of day.
</commit_message>
<xml_diff>
--- a/Harga-PM-H-Heri-Garut.xlsx
+++ b/Harga-PM-H-Heri-Garut.xlsx
@@ -613,23 +613,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
+      <selection pane="bottomRight" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="4" max="4" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1418,7 +1421,7 @@
       <c r="C38" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="3">
         <v>8500</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -1568,8 +1571,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H44"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="80" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>